<commit_message>
Workers and updated rails
</commit_message>
<xml_diff>
--- a/Tablas.xlsx
+++ b/Tablas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaellara/code/projects/admin_sys/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaellara/Desktop/admin-system/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="48000" yWindow="-3140" windowWidth="19200" windowHeight="20180" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="V42" sqref="V42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,24 +833,18 @@
     <col min="3" max="3" width="3.83203125" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.1640625" customWidth="1"/>
-    <col min="17" max="17" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.6640625" customWidth="1"/>
-    <col min="19" max="19" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.5" customWidth="1"/>
-    <col min="21" max="21" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.5" customWidth="1"/>
-    <col min="23" max="23" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.33203125" customWidth="1"/>
+    <col min="13" max="14" width="13" customWidth="1"/>
+    <col min="15" max="16" width="14.1640625" customWidth="1"/>
+    <col min="17" max="18" width="24.6640625" customWidth="1"/>
+    <col min="19" max="20" width="15.5" customWidth="1"/>
+    <col min="21" max="22" width="17.5" customWidth="1"/>
+    <col min="23" max="24" width="15.33203125" customWidth="1"/>
     <col min="25" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14.83203125" bestFit="1" customWidth="1"/>

</xml_diff>